<commit_message>
KAIZEN > Typescript > Getting Started
</commit_message>
<xml_diff>
--- a/Typescript/Typescript.xlsx
+++ b/Typescript/Typescript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\KAIZEN\Typescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC0C576D-B52E-45A2-9312-4894971FA445}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045E171F-D0C0-4732-99C8-3BD2DC1DDA8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
   <si>
     <t>Typescript</t>
   </si>
@@ -371,7 +371,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -381,6 +381,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -413,15 +419,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -709,7 +717,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,13 +731,16 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>2</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -810,9 +821,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/17751414?start=0 - overview" xr:uid="{6470A7AC-6209-4FE1-9551-49EEA14BEC9A}"/>
+    <hyperlink ref="B2" r:id="rId2" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/17751414?start=0 - overview" xr:uid="{A7EFE1D9-B2C6-43E7-B7A5-60F6B186FD75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -835,15 +847,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
KAIZEN > Typescripts > Basics and Types
</commit_message>
<xml_diff>
--- a/Typescript/Typescript.xlsx
+++ b/Typescript/Typescript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\KAIZEN\Typescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045E171F-D0C0-4732-99C8-3BD2DC1DDA8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B882DBE8-9A01-41F1-9842-1115E92CA365}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="97">
   <si>
     <t>Typescript</t>
   </si>
@@ -311,6 +311,12 @@
   </si>
   <si>
     <t>Nightly Builds</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/understanding-typescript/learn/lecture/16888052#overview</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/understanding-typescript/learn/lecture/16888156#overview</t>
   </si>
 </sst>
 </file>
@@ -343,15 +349,6 @@
     </font>
     <font>
       <b/>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -366,6 +363,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -391,7 +396,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -414,22 +419,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -717,7 +754,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,29 +765,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9"/>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="10" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -819,12 +860,16 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/17751414?start=0 - overview" xr:uid="{6470A7AC-6209-4FE1-9551-49EEA14BEC9A}"/>
-    <hyperlink ref="B2" r:id="rId2" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/17751414?start=0 - overview" xr:uid="{A7EFE1D9-B2C6-43E7-B7A5-60F6B186FD75}"/>
+    <hyperlink ref="B2" r:id="rId1" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/17751414?start=0 - overview" xr:uid="{A7EFE1D9-B2C6-43E7-B7A5-60F6B186FD75}"/>
+    <hyperlink ref="B3" r:id="rId2" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/16888052 - overview" xr:uid="{FAD9A0C9-62F9-465B-9E85-0EAC72E9DBD4}"/>
+    <hyperlink ref="B4" r:id="rId3" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/16888156 - overview" xr:uid="{2E3602AC-0941-40F1-9942-17FBF20D75BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -847,15 +892,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
KAIZEN > Typescript > Nextgen Javascript
</commit_message>
<xml_diff>
--- a/Typescript/Typescript.xlsx
+++ b/Typescript/Typescript.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\KAIZEN\Typescript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12A4067-35BE-45FB-993A-5E171A0F2E09}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF5FC2F-6362-457D-9A7E-36B0581373DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="99">
   <si>
     <t>Typescript</t>
   </si>
@@ -320,6 +320,9 @@
   </si>
   <si>
     <t>https://www.udemy.com/course/understanding-typescript/learn/lecture/16888222#overview</t>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/understanding-typescript/learn/lecture/16888240#overview</t>
   </si>
 </sst>
 </file>
@@ -757,7 +760,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:B5"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,13 +770,13 @@
     <col min="3" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="11"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="6" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -781,7 +784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
@@ -789,7 +792,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
@@ -797,17 +800,20 @@
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -874,9 +880,10 @@
     <hyperlink ref="B3" r:id="rId2" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/16888052 - overview" xr:uid="{FAD9A0C9-62F9-465B-9E85-0EAC72E9DBD4}"/>
     <hyperlink ref="B4" r:id="rId3" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/16888156 - overview" xr:uid="{2E3602AC-0941-40F1-9942-17FBF20D75BE}"/>
     <hyperlink ref="B5" r:id="rId4" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/16888222 - overview" xr:uid="{96150571-745E-43BF-BC66-B8A16F01C530}"/>
+    <hyperlink ref="B6" r:id="rId5" location="overview" display="https://www.udemy.com/course/understanding-typescript/learn/lecture/16888240 - overview" xr:uid="{C2099AD0-B8E2-4F8A-8034-D3F56EA545A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>